<commit_message>
added size data for 1/28 resazurin
</commit_message>
<xml_diff>
--- a/data/resazurin/metadata/metadata.xlsx
+++ b/data/resazurin/metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/polyIC-larvae/data/resazurin/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31C1113-1ACE-3D4F-9FCA-ABD373AB2282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40BE231-4FD9-6441-B27A-2471F7811A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32080" yWindow="-80" windowWidth="28040" windowHeight="17440" xr2:uid="{F9B76D48-E646-9D48-9AB8-3319F507EDF2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F9B76D48-E646-9D48-9AB8-3319F507EDF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7159BF13-8618-0540-AFAB-AF0D60C37565}">
   <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
-      <selection activeCell="F377" sqref="F377"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4704,16 +4704,16 @@
         <v>112</v>
       </c>
       <c r="E151" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F151" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G151" t="s">
         <v>65</v>
       </c>
       <c r="H151" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added size normalized analysis
</commit_message>
<xml_diff>
--- a/data/resazurin/metadata/metadata.xlsx
+++ b/data/resazurin/metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/polyIC-larvae/data/resazurin/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40BE231-4FD9-6441-B27A-2471F7811A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A5C8A1-3997-3C41-AD19-6491193159F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F9B76D48-E646-9D48-9AB8-3319F507EDF2}"/>
+    <workbookView xWindow="500" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F9B76D48-E646-9D48-9AB8-3319F507EDF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7159BF13-8618-0540-AFAB-AF0D60C37565}">
   <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G157" sqref="G157"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1893,19 +1893,19 @@
         <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G43" t="s">
         <v>53</v>
       </c>
       <c r="H43" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -2205,19 +2205,19 @@
         <v>108</v>
       </c>
       <c r="D55" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F55" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G55" t="s">
         <v>65</v>
       </c>
       <c r="H55" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -4392,16 +4392,16 @@
         <v>112</v>
       </c>
       <c r="E139" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F139" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G139" t="s">
         <v>53</v>
       </c>
       <c r="H139" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -4415,7 +4415,7 @@
         <v>108</v>
       </c>
       <c r="D140" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E140" t="s">
         <v>110</v>
@@ -4441,7 +4441,7 @@
         <v>108</v>
       </c>
       <c r="D141" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E141" t="s">
         <v>110</v>
@@ -4467,7 +4467,7 @@
         <v>108</v>
       </c>
       <c r="D142" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E142" t="s">
         <v>110</v>
@@ -4493,7 +4493,7 @@
         <v>108</v>
       </c>
       <c r="D143" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E143" t="s">
         <v>110</v>
@@ -4519,7 +4519,7 @@
         <v>108</v>
       </c>
       <c r="D144" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E144" t="s">
         <v>110</v>
@@ -4545,7 +4545,7 @@
         <v>108</v>
       </c>
       <c r="D145" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E145" t="s">
         <v>110</v>
@@ -4571,7 +4571,7 @@
         <v>108</v>
       </c>
       <c r="D146" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E146" t="s">
         <v>110</v>
@@ -4597,7 +4597,7 @@
         <v>108</v>
       </c>
       <c r="D147" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E147" t="s">
         <v>110</v>
@@ -4623,7 +4623,7 @@
         <v>108</v>
       </c>
       <c r="D148" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E148" t="s">
         <v>110</v>
@@ -4649,7 +4649,7 @@
         <v>108</v>
       </c>
       <c r="D149" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E149" t="s">
         <v>110</v>
@@ -4675,7 +4675,7 @@
         <v>108</v>
       </c>
       <c r="D150" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E150" t="s">
         <v>110</v>
@@ -4701,19 +4701,19 @@
         <v>108</v>
       </c>
       <c r="D151" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E151" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F151" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G151" t="s">
         <v>65</v>
       </c>
       <c r="H151" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -6885,19 +6885,19 @@
         <v>116</v>
       </c>
       <c r="D235" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="E235" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F235" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G235" t="s">
         <v>53</v>
       </c>
       <c r="H235" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
@@ -9384,16 +9384,16 @@
         <v>112</v>
       </c>
       <c r="E331" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F331" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G331" t="s">
         <v>53</v>
       </c>
       <c r="H331" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.2">
@@ -9407,7 +9407,7 @@
         <v>116</v>
       </c>
       <c r="D332" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E332" t="s">
         <v>110</v>
@@ -9433,7 +9433,7 @@
         <v>116</v>
       </c>
       <c r="D333" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E333" t="s">
         <v>110</v>
@@ -9459,7 +9459,7 @@
         <v>116</v>
       </c>
       <c r="D334" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E334" t="s">
         <v>110</v>
@@ -9485,7 +9485,7 @@
         <v>116</v>
       </c>
       <c r="D335" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E335" t="s">
         <v>110</v>
@@ -9511,7 +9511,7 @@
         <v>116</v>
       </c>
       <c r="D336" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E336" t="s">
         <v>110</v>
@@ -9537,7 +9537,7 @@
         <v>116</v>
       </c>
       <c r="D337" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E337" t="s">
         <v>110</v>
@@ -9563,7 +9563,7 @@
         <v>116</v>
       </c>
       <c r="D338" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E338" t="s">
         <v>110</v>
@@ -9589,7 +9589,7 @@
         <v>116</v>
       </c>
       <c r="D339" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E339" t="s">
         <v>110</v>
@@ -9615,7 +9615,7 @@
         <v>116</v>
       </c>
       <c r="D340" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E340" t="s">
         <v>110</v>
@@ -9641,7 +9641,7 @@
         <v>116</v>
       </c>
       <c r="D341" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E341" t="s">
         <v>110</v>
@@ -9667,7 +9667,7 @@
         <v>116</v>
       </c>
       <c r="D342" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E342" t="s">
         <v>110</v>
@@ -9693,7 +9693,7 @@
         <v>116</v>
       </c>
       <c r="D343" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E343" t="s">
         <v>110</v>

</xml_diff>